<commit_message>
total_ontologies excel file updated
</commit_message>
<xml_diff>
--- a/excel_files/total_ontologies.xlsx
+++ b/excel_files/total_ontologies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">AgroPortal</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">vocab.deri.ie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfdata.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swoogle.umbc.edu(counting)</t>
   </si>
 </sst>
 </file>
@@ -65,11 +71,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="15">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -87,51 +94,85 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -232,22 +273,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -347,10 +420,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="93" zoomScaleNormal="93" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,6 +439,9 @@
       <c r="B1" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="C1" s="0" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -453,6 +529,25 @@
       </c>
       <c r="B12" s="0" t="n">
         <v>82</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1202</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>